<commit_message>
configured cpu/cuda dat mapping
</commit_message>
<xml_diff>
--- a/logs/pruning_stats.xlsx
+++ b/logs/pruning_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/zixian_jin_intel_com/Documents/FYP/mase-pruning-test/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="11_F25DC773A252ABDACC1048F4B15A5A3A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4514BB17-B743-46BF-91B9-8A3F8308AF50}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="11_F25DC773A252ABDACC1048F4B15A5A3A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9CBEE1C-1D49-4861-AA64-3CA9A62FF8DE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>model.fc1: Linear(320, 50)</t>
   </si>
@@ -48,10 +48,25 @@
     <t>Using pretrained model. Pre-pruning validation acc. = 98.01%, validation loss=0.05974</t>
   </si>
   <si>
-    <t>Pruning After Training</t>
-  </si>
-  <si>
-    <t>Pruning with Training</t>
+    <t>val acc after 5 epochs</t>
+  </si>
+  <si>
+    <t>Structured Pruning After Training</t>
+  </si>
+  <si>
+    <t>Structured Pruning with Training</t>
+  </si>
+  <si>
+    <t>97.91% -&gt; 11.35%</t>
+  </si>
+  <si>
+    <t>97.83% -&gt; 95.57%</t>
+  </si>
+  <si>
+    <t>97.87% -&gt; 96.93%</t>
+  </si>
+  <si>
+    <t>97.73% -&gt; 97.69%</t>
   </si>
 </sst>
 </file>
@@ -138,6 +153,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,8 +437,9 @@
     <col min="5" max="5" width="8.88671875" style="1"/>
     <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
     <col min="7" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="11.21875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="13.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.88671875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -438,12 +458,12 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -474,7 +494,7 @@
         <v>2</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>4</v>
@@ -503,7 +523,7 @@
         <v>0.04</v>
       </c>
       <c r="J5" s="3">
-        <v>0.97409999999999997</v>
+        <v>0.97970000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -529,7 +549,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="J6" s="3">
-        <v>0.97370000000000001</v>
+        <v>0.98060000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -555,7 +575,7 @@
         <v>0.06</v>
       </c>
       <c r="J7" s="3">
-        <v>0.96009999999999995</v>
+        <v>0.97829999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -581,7 +601,7 @@
         <v>0.08</v>
       </c>
       <c r="J8" s="3">
-        <v>0.95579999999999998</v>
+        <v>0.97950000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -607,7 +627,7 @@
         <v>0.01</v>
       </c>
       <c r="J9" s="3">
-        <v>0.92269999999999996</v>
+        <v>0.98199999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -633,7 +653,7 @@
         <v>0.2</v>
       </c>
       <c r="J10" s="3">
-        <v>0.1135</v>
+        <v>0.97740000000000005</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -655,9 +675,7 @@
       <c r="H12" s="1">
         <v>0.5</v>
       </c>
-      <c r="J12" s="3">
-        <v>0.97509999999999997</v>
-      </c>
+      <c r="J12" s="3"/>
       <c r="K12" s="1">
         <v>0.13880000000000001</v>
       </c>
@@ -681,9 +699,7 @@
       <c r="H13" s="1">
         <v>0.6</v>
       </c>
-      <c r="J13" s="3">
-        <v>0.96750000000000003</v>
-      </c>
+      <c r="J13" s="3"/>
       <c r="K13" s="1">
         <v>0.22770000000000001</v>
       </c>
@@ -707,8 +723,8 @@
       <c r="H14" s="1">
         <v>0.7</v>
       </c>
-      <c r="J14" s="3">
-        <v>0.97009999999999996</v>
+      <c r="J14" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="K14" s="1">
         <v>0.36049999999999999</v>
@@ -733,8 +749,8 @@
       <c r="H15" s="1">
         <v>0.8</v>
       </c>
-      <c r="J15" s="3">
-        <v>0.95440000000000003</v>
+      <c r="J15" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="K15" s="1">
         <v>0.72950000000000004</v>
@@ -759,8 +775,8 @@
       <c r="H16" s="1">
         <v>0.9</v>
       </c>
-      <c r="J16" s="3">
-        <v>0.9113</v>
+      <c r="J16" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="K16" s="1">
         <v>1.2361</v>
@@ -785,8 +801,8 @@
       <c r="H17" s="1">
         <v>1</v>
       </c>
-      <c r="J17" s="3">
-        <v>0.1135</v>
+      <c r="J17" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="K17" s="1">
         <v>2.3068</v>
@@ -808,9 +824,7 @@
       <c r="H19" s="1">
         <v>0.5</v>
       </c>
-      <c r="J19" s="3">
-        <v>0.97629999999999995</v>
-      </c>
+      <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -828,9 +842,7 @@
       <c r="H20" s="1">
         <v>0.6</v>
       </c>
-      <c r="J20" s="3">
-        <v>0.97550000000000003</v>
-      </c>
+      <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -849,7 +861,7 @@
         <v>0.7</v>
       </c>
       <c r="J21" s="3">
-        <v>0.96950000000000003</v>
+        <v>0.98040000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -869,7 +881,7 @@
         <v>0.8</v>
       </c>
       <c r="J22" s="3">
-        <v>0.96430000000000005</v>
+        <v>0.97940000000000005</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -888,9 +900,7 @@
       <c r="H23" s="1">
         <v>0.9</v>
       </c>
-      <c r="J23" s="3">
-        <v>0.9415</v>
-      </c>
+      <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -908,9 +918,7 @@
       <c r="H24" s="1">
         <v>1</v>
       </c>
-      <c r="J24" s="3">
-        <v>0.1135</v>
-      </c>
+      <c r="J24" s="3"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -928,9 +936,7 @@
       <c r="H26" s="1">
         <v>0.5</v>
       </c>
-      <c r="J26" s="3">
-        <v>0.97650000000000003</v>
-      </c>
+      <c r="J26" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -948,9 +954,7 @@
       <c r="H27" s="1">
         <v>0.6</v>
       </c>
-      <c r="J27" s="3">
-        <v>0.97650000000000003</v>
-      </c>
+      <c r="J27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -968,9 +972,7 @@
       <c r="H28" s="1">
         <v>0.7</v>
       </c>
-      <c r="J28" s="3">
-        <v>0.97509999999999997</v>
-      </c>
+      <c r="J28" s="3"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -988,9 +990,7 @@
       <c r="H29" s="1">
         <v>0.8</v>
       </c>
-      <c r="J29" s="3">
-        <v>0.96970000000000001</v>
-      </c>
+      <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
@@ -1008,9 +1008,7 @@
       <c r="H30" s="1">
         <v>0.9</v>
       </c>
-      <c r="J30" s="3">
-        <v>0.95979999999999999</v>
-      </c>
+      <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
@@ -1028,9 +1026,7 @@
       <c r="H31" s="1">
         <v>1</v>
       </c>
-      <c r="J31" s="3">
-        <v>0.1135</v>
-      </c>
+      <c r="J31" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
updated stats: l layers & all weights pruned
</commit_message>
<xml_diff>
--- a/logs/pruning_stats.xlsx
+++ b/logs/pruning_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/zixian_jin_intel_com/Documents/FYP/mase-pruning-test/logs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/cj323_ic_ac_uk/Documents/FYP/mase-pruning-test/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="536" documentId="11_F25DC773A252ABDACC1048F4B15A5A3A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F3CB2C5-B9FF-431E-8BD5-695CBAED176D}"/>
+  <xr:revisionPtr revIDLastSave="554" documentId="11_F25DC773A252ABDACC1048F4B15A5A3A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D1896C2-C3BE-4B98-AD34-83749772123A}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-98" windowWidth="28995" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MNIST_CNN" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="40">
   <si>
     <t>model.fc1: Linear(320, 50)</t>
   </si>
@@ -144,16 +144,20 @@
   <si>
     <t xml:space="preserve">All trials are of post-training pruning. Pre-Training Acc. = 87.395%. </t>
   </si>
+  <si>
+    <t>All Layers</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -161,7 +165,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -169,14 +173,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -184,15 +188,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -251,15 +262,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -287,12 +289,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -302,10 +298,25 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -329,7 +340,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -391,7 +402,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -666,7 +677,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -821,7 +831,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-CN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -859,7 +869,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1096624768"/>
@@ -941,7 +951,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-CN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -973,7 +983,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1096626208"/>
@@ -1015,7 +1025,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1052,7 +1062,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1066,641 +1076,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>Multiple Layers, All Weights (QKV)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Odd Layers (1 3 5 7 9)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="4"/>
-              <c:pt idx="0">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>3</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>4</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>5</c:v>
-              </c:pt>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
-                </c:ext>
-              </c:extLst>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'BERT-Base'!$L$21:$L$25</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'BERT-Base'!$L$22:$L$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>87.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>87.08</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>82.91</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>83.75</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-13D9-488B-A566-6D2AECED20F4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Even Layers (2 4 6 8 10)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="4"/>
-              <c:pt idx="0">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>3</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>4</c:v>
-              </c:pt>
-              <c:pt idx="3">
-                <c:v>5</c:v>
-              </c:pt>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
-                </c:ext>
-              </c:extLst>
-            </c:strLit>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'BERT-Base'!$M$21:$M$25</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'BERT-Base'!$M$22:$M$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>88.02</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>88.02</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>87.19</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>86.35</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-13D9-488B-A566-6D2AECED20F4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1179468464"/>
-        <c:axId val="1179468944"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="0"/>
-                <c:spPr>
-                  <a:ln w="28575" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent1"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:fullRef>
-                          <c15:sqref>'BERT-Base'!$K$21:$K$25</c15:sqref>
-                        </c15:fullRef>
-                        <c15:formulaRef>
-                          <c15:sqref>'BERT-Base'!$K$22:$K$25</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="4"/>
-                      <c:pt idx="0">
-                        <c:v>0.5</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0.6</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.7</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.8</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-13D9-488B-A566-6D2AECED20F4}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
-          </c:ext>
-        </c:extLst>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1179468464"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="zh-CN"/>
-                  <a:t>Sparsity</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1179468944"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1179468944"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Acc</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1179468464"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1775,7 +1151,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1842,7 +1218,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1987,7 +1363,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -2132,7 +1508,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -2290,7 +1666,7 @@
                           <a:cs typeface="+mn-cs"/>
                         </a:defRPr>
                       </a:pPr>
-                      <a:endParaRPr lang="en-US"/>
+                      <a:endParaRPr lang="zh-CN"/>
                     </a:p>
                   </c:txPr>
                   <c:dLblPos val="t"/>
@@ -2420,7 +1796,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-CN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2458,7 +1834,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="338166624"/>
@@ -2540,7 +1916,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-CN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2572,7 +1948,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="338169504"/>
@@ -2614,7 +1990,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2651,7 +2027,571 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Multiple</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t> Layers, All Weights (QKV)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'BERT-Base'!$L$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Odd Layers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'BERT-Base'!$L$22:$L$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>87.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87.08</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.91</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FBEC-4BA6-8B05-9634AD60453D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'BERT-Base'!$M$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Even Layers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'BERT-Base'!$M$22:$M$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>88.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FBEC-4BA6-8B05-9634AD60453D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'BERT-Base'!$N$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>All Layers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'BERT-Base'!$N$22:$N$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>67.92</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FBEC-4BA6-8B05-9634AD60453D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1082056815"/>
+        <c:axId val="1082061135"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'BERT-Base'!$K$21</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Acc</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'BERT-Base'!$K$22:$K$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.6</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.7</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.8</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-FBEC-4BA6-8B05-9634AD60453D}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1082056815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1082061135"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1082061135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1082056815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4332,42 +4272,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>141445</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>150494</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>446245</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>172402</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6E80C3B-839C-7400-0842-4C2A13D88F44}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
       <xdr:colOff>6191</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>32384</xdr:rowOff>
@@ -4395,6 +4299,42 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5535775D-04CF-6954-9CC4-68F7241CE590}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
@@ -4402,10 +4342,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4677,7 +4613,7 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.21875" style="1" customWidth="1"/>
@@ -4691,33 +4627,33 @@
     <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="5" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="G3" s="5" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="G3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" s="2" customFormat="1">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -4749,7 +4685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4775,7 +4711,7 @@
         <v>0.97970000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4801,7 +4737,7 @@
         <v>0.98060000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -4827,7 +4763,7 @@
         <v>0.97829999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -4853,7 +4789,7 @@
         <v>0.97950000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -4879,7 +4815,7 @@
         <v>0.98199999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -4905,7 +4841,7 @@
         <v>0.97740000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -4929,7 +4865,7 @@
         <v>0.13880000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -4953,7 +4889,7 @@
         <v>0.22770000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -4979,7 +4915,7 @@
         <v>0.36049999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>8</v>
       </c>
@@ -5005,7 +4941,7 @@
         <v>0.72950000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -5031,7 +4967,7 @@
         <v>1.2361</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -5057,7 +4993,7 @@
         <v>2.3068</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>20</v>
       </c>
@@ -5075,7 +5011,7 @@
       </c>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -5093,7 +5029,7 @@
       </c>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -5113,7 +5049,7 @@
         <v>0.98040000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -5133,7 +5069,7 @@
         <v>0.97940000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -5151,7 +5087,7 @@
       </c>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -5169,7 +5105,7 @@
       </c>
       <c r="J24" s="3"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>40</v>
       </c>
@@ -5187,7 +5123,7 @@
       </c>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>40</v>
       </c>
@@ -5205,7 +5141,7 @@
       </c>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>40</v>
       </c>
@@ -5223,7 +5159,7 @@
       </c>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>40</v>
       </c>
@@ -5241,7 +5177,7 @@
       </c>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>40</v>
       </c>
@@ -5259,7 +5195,7 @@
       </c>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>40</v>
       </c>
@@ -5284,6 +5220,7 @@
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="A1:B1"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5291,45 +5228,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55651361-8A1C-4838-B592-C2F6F1279844}">
-  <dimension ref="A1:R57"/>
+  <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="8"/>
+    <col min="4" max="4" width="8.88671875" style="5"/>
     <col min="5" max="5" width="10.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.88671875" style="1" customWidth="1"/>
     <col min="7" max="11" width="8.88671875" style="1"/>
     <col min="12" max="12" width="11.33203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="11.77734375" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="9.6640625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="K2" s="15" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-    </row>
-    <row r="3" spans="1:15" s="2" customFormat="1">
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -5339,7 +5277,7 @@
       <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -5348,880 +5286,894 @@
       <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="12">
         <v>0</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="12">
         <v>3</v>
       </c>
-      <c r="N3" s="16">
+      <c r="N3" s="12">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="9">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>0</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="16">
         <v>64</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="7">
         <v>0.9</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <v>87.4</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="6">
         <v>89.27</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="12">
         <v>0.9</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="6">
         <v>89.27</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="6">
         <v>89.06</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="6">
         <v>87.6</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="9">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>0</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10">
+      <c r="C5" s="6"/>
+      <c r="D5" s="7">
         <v>0.95</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
         <v>89.06</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="12">
         <v>0.95</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="6">
         <v>89.06</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="6">
         <v>90.1</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="6">
         <v>87.19</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="9">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>0</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10">
+      <c r="C6" s="6"/>
+      <c r="D6" s="7">
         <v>0.98</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6">
         <v>88.85</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="12">
         <v>0.98</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="6">
         <v>88.85</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="6">
         <v>88.02</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="6">
         <v>88.02</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="9">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>0</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10">
+      <c r="C7" s="6"/>
+      <c r="D7" s="7">
         <v>1</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6">
         <v>89.58</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="12">
         <v>1</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L7" s="6">
         <v>89.58</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="6">
         <v>89.27</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="6">
         <v>87.29</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="9">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>3</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10">
+      <c r="C9" s="6"/>
+      <c r="D9" s="7">
         <v>0.9</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6">
         <v>89.06</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="9">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>3</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10">
+      <c r="C10" s="6"/>
+      <c r="D10" s="7">
         <v>0.95</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6">
         <v>90.1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="9">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>3</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10">
+      <c r="C11" s="6"/>
+      <c r="D11" s="7">
         <v>0.98</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6">
         <v>88.02</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="13"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="9">
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="10"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>3</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10">
+      <c r="C12" s="6"/>
+      <c r="D12" s="7">
         <v>1</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9">
+      <c r="E12" s="6"/>
+      <c r="F12" s="6">
         <v>89.27</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="L12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="18" t="s">
+      <c r="M12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="N12" s="18" t="s">
+      <c r="N12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="O12" s="18" t="s">
+      <c r="O12" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="K13" s="18">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="K13" s="13">
         <v>0.5</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="10">
         <v>88.23</v>
       </c>
-      <c r="M13" s="13">
+      <c r="M13" s="10">
         <v>88.23</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13" s="14">
         <v>86.56</v>
       </c>
-      <c r="O13" s="13">
+      <c r="O13" s="10">
         <v>88.96</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="9">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>11</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10">
+      <c r="C14" s="6"/>
+      <c r="D14" s="7">
         <v>0.9</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6">
         <v>87.6</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="13">
         <v>0.6</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="10">
         <v>78.540000000000006</v>
       </c>
-      <c r="M14" s="13">
+      <c r="M14" s="10">
         <v>84.79</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="14">
         <v>86.25</v>
       </c>
-      <c r="O14" s="13">
+      <c r="O14" s="10">
         <v>87.92</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="9">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <v>11</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10">
+      <c r="C15" s="6"/>
+      <c r="D15" s="7">
         <v>0.95</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9">
+      <c r="E15" s="6"/>
+      <c r="F15" s="6">
         <v>87.19</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="13">
         <v>0.7</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="10">
         <v>66.86</v>
       </c>
-      <c r="M15" s="13">
+      <c r="M15" s="10">
         <v>74.900000000000006</v>
       </c>
-      <c r="N15" s="19">
+      <c r="N15" s="14">
         <v>85</v>
       </c>
-      <c r="O15" s="13">
+      <c r="O15" s="10">
         <v>86.46</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="9">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
         <v>11</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10">
+      <c r="C16" s="6"/>
+      <c r="D16" s="7">
         <v>0.98</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6">
         <v>88.02</v>
       </c>
-      <c r="K16" s="18">
+      <c r="K16" s="13">
         <v>0.8</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="10">
         <v>60</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="10">
         <v>60</v>
       </c>
-      <c r="N16" s="19">
+      <c r="N16" s="14">
         <v>79.38</v>
       </c>
-      <c r="O16" s="13">
+      <c r="O16" s="10">
         <v>85.73</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="9">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
         <v>11</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10">
+      <c r="C17" s="6"/>
+      <c r="D17" s="7">
         <v>1</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6">
         <v>87.29</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1"/>
-    <row r="20" spans="1:15">
-      <c r="K20" s="20" t="s">
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K20" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="11"/>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="13" t="s">
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="8"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14">
+      <c r="C21" s="10"/>
+      <c r="D21" s="11">
         <v>0.5</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13">
+      <c r="E21" s="10"/>
+      <c r="F21" s="10">
         <v>88.23</v>
       </c>
-      <c r="K21" s="21" t="s">
+      <c r="K21" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="L21" s="21" t="s">
+      <c r="L21" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="M21" s="21" t="s">
+      <c r="M21" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="N21" s="21"/>
-      <c r="O21" s="11"/>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="A22" s="13" t="s">
+      <c r="N21" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" s="8"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14">
+      <c r="C22" s="10"/>
+      <c r="D22" s="11">
         <v>0.6</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13">
+      <c r="E22" s="10"/>
+      <c r="F22" s="10">
         <v>78.540000000000006</v>
       </c>
-      <c r="K22" s="21">
+      <c r="K22" s="15">
         <v>0.5</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="8">
         <v>87.4</v>
       </c>
-      <c r="M22" s="11">
+      <c r="M22" s="8">
         <v>88.02</v>
       </c>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="13" t="s">
+      <c r="N22" s="8">
+        <v>67.92</v>
+      </c>
+      <c r="O22" s="8"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14">
+      <c r="C23" s="10"/>
+      <c r="D23" s="11">
         <v>0.7</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13">
+      <c r="E23" s="10"/>
+      <c r="F23" s="10">
         <v>66.86</v>
       </c>
-      <c r="K23" s="21">
+      <c r="K23" s="15">
         <v>0.6</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="8">
         <v>87.08</v>
       </c>
-      <c r="M23" s="11">
+      <c r="M23" s="8">
         <v>88.02</v>
       </c>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-    </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="K24" s="21">
+      <c r="N23" s="8">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="O23" s="8"/>
+    </row>
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="K24" s="15">
         <v>0.7</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="8">
         <v>82.91</v>
       </c>
-      <c r="M24" s="11">
+      <c r="M24" s="8">
         <v>87.19</v>
       </c>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="13" t="s">
+      <c r="N24" s="8">
+        <v>62.81</v>
+      </c>
+      <c r="O24" s="8"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="14">
+      <c r="C25" s="10"/>
+      <c r="D25" s="11">
         <v>0.5</v>
       </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13">
+      <c r="E25" s="10"/>
+      <c r="F25" s="10">
         <v>88.23</v>
       </c>
-      <c r="K25" s="21">
+      <c r="K25" s="15">
         <v>0.8</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="8">
         <v>83.75</v>
       </c>
-      <c r="M25" s="11">
+      <c r="M25" s="8">
         <v>86.35</v>
       </c>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="13" t="s">
+      <c r="N25" s="8">
+        <v>53.96</v>
+      </c>
+      <c r="O25" s="8"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14">
+      <c r="C26" s="10"/>
+      <c r="D26" s="11">
         <v>0.6</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13">
+      <c r="E26" s="10"/>
+      <c r="F26" s="10">
         <v>84.79</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14">
+      <c r="C27" s="10"/>
+      <c r="D27" s="11">
         <v>0.7</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13">
+      <c r="E27" s="10"/>
+      <c r="F27" s="10">
         <v>74.900000000000006</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="13" t="s">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14">
+      <c r="C29" s="10"/>
+      <c r="D29" s="11">
         <v>0.5</v>
       </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13">
+      <c r="E29" s="10"/>
+      <c r="F29" s="10">
         <v>88.96</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
-      <c r="A30" s="13" t="s">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14">
+      <c r="C30" s="10"/>
+      <c r="D30" s="11">
         <v>0.6</v>
       </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13">
+      <c r="E30" s="10"/>
+      <c r="F30" s="10">
         <v>87.92</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="13" t="s">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14">
+      <c r="C31" s="10"/>
+      <c r="D31" s="11">
         <v>0.7</v>
       </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13">
+      <c r="E31" s="10"/>
+      <c r="F31" s="10">
         <v>86.46</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="13" t="s">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14">
+      <c r="C32" s="10"/>
+      <c r="D32" s="11">
         <v>0.8</v>
       </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13">
+      <c r="E32" s="10"/>
+      <c r="F32" s="10">
         <v>85.73</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-    </row>
-    <row r="34" spans="1:18">
-      <c r="A34" s="13" t="s">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13">
+      <c r="C34" s="10"/>
+      <c r="D34" s="10">
         <v>0.5</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13">
+      <c r="E34" s="10"/>
+      <c r="F34" s="10">
         <v>86.56</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
-      <c r="A35" s="13" t="s">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13">
+      <c r="C35" s="10"/>
+      <c r="D35" s="10">
         <v>0.6</v>
       </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13">
+      <c r="E35" s="10"/>
+      <c r="F35" s="10">
         <v>86.25</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
-      <c r="A36" s="13" t="s">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13">
+      <c r="C36" s="10"/>
+      <c r="D36" s="10">
         <v>0.7</v>
       </c>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13">
+      <c r="E36" s="10"/>
+      <c r="F36" s="10">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
-      <c r="A37" s="13" t="s">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13">
+      <c r="C37" s="10"/>
+      <c r="D37" s="10">
         <v>0.8</v>
       </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13">
+      <c r="E37" s="10"/>
+      <c r="F37" s="10">
         <v>79.38</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
-      <c r="A41" s="11" t="s">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="12">
+      <c r="C41" s="8"/>
+      <c r="D41" s="9">
         <v>0.5</v>
       </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11">
+      <c r="E41" s="8"/>
+      <c r="F41" s="8">
         <v>87.4</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
-      <c r="A42" s="11" t="s">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="12">
+      <c r="C42" s="8"/>
+      <c r="D42" s="9">
         <v>0.6</v>
       </c>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11">
+      <c r="E42" s="8"/>
+      <c r="F42" s="8">
         <v>87.08</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
-      <c r="A43" s="11" t="s">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="12">
+      <c r="C43" s="8"/>
+      <c r="D43" s="9">
         <v>0.7</v>
       </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11">
+      <c r="E43" s="8"/>
+      <c r="F43" s="8">
         <v>82.91</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
-      <c r="A44" s="11" t="s">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="12">
+      <c r="C44" s="8"/>
+      <c r="D44" s="9">
         <v>0.8</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11">
+      <c r="E44" s="8"/>
+      <c r="F44" s="8">
         <v>83.75</v>
       </c>
-      <c r="R44" s="8"/>
-    </row>
-    <row r="45" spans="1:18">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="R45" s="8"/>
-    </row>
-    <row r="46" spans="1:18">
-      <c r="A46" s="11" t="s">
+      <c r="R44" s="5"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="R45" s="5"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="12">
+      <c r="C46" s="8"/>
+      <c r="D46" s="9">
         <v>0.5</v>
       </c>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11">
+      <c r="E46" s="8"/>
+      <c r="F46" s="8">
         <v>88.02</v>
       </c>
-      <c r="R46" s="8"/>
-    </row>
-    <row r="47" spans="1:18">
-      <c r="A47" s="11" t="s">
+      <c r="R46" s="5"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="12">
+      <c r="C47" s="8"/>
+      <c r="D47" s="9">
         <v>0.6</v>
       </c>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11">
+      <c r="E47" s="8"/>
+      <c r="F47" s="8">
         <v>88.02</v>
       </c>
-      <c r="R47" s="8"/>
-    </row>
-    <row r="48" spans="1:18">
-      <c r="A48" s="11" t="s">
+      <c r="R47" s="5"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="12">
+      <c r="C48" s="8"/>
+      <c r="D48" s="9">
         <v>0.7</v>
       </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11">
+      <c r="E48" s="8"/>
+      <c r="F48" s="8">
         <v>87.19</v>
       </c>
     </row>
-    <row r="49" spans="1:6" customFormat="1">
-      <c r="A49" s="11" t="s">
+    <row r="49" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="12">
+      <c r="C49" s="8"/>
+      <c r="D49" s="9">
         <v>0.8</v>
       </c>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11">
+      <c r="E49" s="8"/>
+      <c r="F49" s="8">
         <v>86.35</v>
       </c>
     </row>
-    <row r="50" spans="1:6" customFormat="1">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" customFormat="1">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="1:6" customFormat="1">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="1" t="s">
+    <row r="50" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B51" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D54" s="8">
+      <c r="C51" s="8"/>
+      <c r="D51" s="9">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="1" t="s">
+      <c r="E51" s="8"/>
+      <c r="F51" s="8">
+        <v>67.92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B52" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D55" s="8">
+      <c r="C52" s="8"/>
+      <c r="D52" s="9">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="1" t="s">
+      <c r="E52" s="8"/>
+      <c r="F52" s="8">
+        <v>67.599999999999994</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B53" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="8">
+      <c r="C53" s="8"/>
+      <c r="D53" s="9">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="1" t="s">
+      <c r="E53" s="8"/>
+      <c r="F53" s="8">
+        <v>62.81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B54" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D57" s="8">
+      <c r="C54" s="8"/>
+      <c r="D54" s="9">
         <v>0.8</v>
+      </c>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8">
+        <v>53.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>